<commit_message>
Updated ScrumbleEvaluation and ETB
</commit_message>
<xml_diff>
--- a/doc/teambuilding/AutovalutazioneScrumble.xlsx
+++ b/doc/teambuilding/AutovalutazioneScrumble.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>GOAL</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Q15</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -794,9 +791,7 @@
     </row>
     <row r="19">
       <c r="E19" s="10"/>
-      <c r="G19" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="G19" s="10"/>
     </row>
     <row r="20">
       <c r="E20" s="10"/>

</xml_diff>